<commit_message>
Included scroll function and included hover over disappearing menu and click on menu item
</commit_message>
<xml_diff>
--- a/src/test/resources/amazonLoginTestData.xlsx
+++ b/src/test/resources/amazonLoginTestData.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">XXXXXXX</t>
+    <t xml:space="preserve">yourUsername</t>
   </si>
   <si>
-    <t xml:space="preserve">XXXXXX</t>
+    <t xml:space="preserve">yourPassword</t>
   </si>
 </sst>
 </file>

</xml_diff>